<commit_message>
fix: Ajusts planilha caio
</commit_message>
<xml_diff>
--- a/data_loader/data/Caio_Banco_de_Horas.xlsx
+++ b/data_loader/data/Caio_Banco_de_Horas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ramonhveloso\projects\erp-automa-back-end\data_loader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCFD7C8-3ABC-4D6A-A7B6-410ED89B7EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1411D27C-E2FE-407E-8EA4-B4116D7BBE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jornadas" sheetId="1" r:id="rId1"/>
@@ -634,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:AA922"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A590" workbookViewId="0">
+      <selection activeCell="J632" sqref="J632"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -21330,8 +21330,8 @@
         <v>40.416666666666664</v>
       </c>
       <c r="J544" s="11">
-        <f>SUM($I$5:I544)</f>
-        <v>35601.458333333343</v>
+        <f>SUM($I$2:I544)</f>
+        <v>35687.333333333336</v>
       </c>
     </row>
     <row r="545" spans="1:10" ht="12.75">
@@ -21368,8 +21368,8 @@
         <v>158.33333333333331</v>
       </c>
       <c r="J545" s="11">
-        <f>SUM($I$5:I545)</f>
-        <v>35759.791666666679</v>
+        <f>SUM($I$2:I545)</f>
+        <v>35845.666666666672</v>
       </c>
     </row>
     <row r="546" spans="1:10" ht="12.75">
@@ -21406,8 +21406,8 @@
         <v>57.499999999999993</v>
       </c>
       <c r="J546" s="11">
-        <f>SUM($I$5:I546)</f>
-        <v>35817.291666666679</v>
+        <f>SUM($I$2:I546)</f>
+        <v>35903.166666666672</v>
       </c>
     </row>
     <row r="547" spans="1:10" ht="12.75">
@@ -21444,8 +21444,8 @@
         <v>61.250000000000007</v>
       </c>
       <c r="J547" s="11">
-        <f>SUM($I$5:I547)</f>
-        <v>35878.541666666679</v>
+        <f>SUM($I$2:I547)</f>
+        <v>35964.416666666672</v>
       </c>
     </row>
     <row r="548" spans="1:10" ht="12.75">
@@ -21482,8 +21482,8 @@
         <v>61.250000000000007</v>
       </c>
       <c r="J548" s="11">
-        <f>SUM($I$5:I548)</f>
-        <v>35939.791666666679</v>
+        <f>SUM($I$2:I548)</f>
+        <v>36025.666666666672</v>
       </c>
     </row>
     <row r="549" spans="1:10" ht="12.75">
@@ -21520,8 +21520,8 @@
         <v>89.166666666666671</v>
       </c>
       <c r="J549" s="11">
-        <f>SUM($I$5:I549)</f>
-        <v>36028.958333333343</v>
+        <f>SUM($I$2:I549)</f>
+        <v>36114.833333333336</v>
       </c>
     </row>
     <row r="550" spans="1:10" ht="12.75">
@@ -21558,8 +21558,8 @@
         <v>104.58333333333334</v>
       </c>
       <c r="J550" s="11">
-        <f>SUM($I$5:I550)</f>
-        <v>36133.541666666679</v>
+        <f>SUM($I$2:I550)</f>
+        <v>36219.416666666672</v>
       </c>
     </row>
     <row r="551" spans="1:10" ht="12.75">
@@ -21596,8 +21596,8 @@
         <v>86.25</v>
       </c>
       <c r="J551" s="11">
-        <f>SUM($I$5:I551)</f>
-        <v>36219.791666666679</v>
+        <f>SUM($I$2:I551)</f>
+        <v>36305.666666666672</v>
       </c>
     </row>
     <row r="552" spans="1:10" ht="12.75">
@@ -21634,8 +21634,8 @@
         <v>93.75</v>
       </c>
       <c r="J552" s="11">
-        <f>SUM($I$5:I552)</f>
-        <v>36313.541666666679</v>
+        <f>SUM($I$2:I552)</f>
+        <v>36399.416666666672</v>
       </c>
     </row>
     <row r="553" spans="1:10" ht="12.75">
@@ -21672,8 +21672,8 @@
         <v>62.5</v>
       </c>
       <c r="J553" s="11">
-        <f>SUM($I$5:I553)</f>
-        <v>36376.041666666679</v>
+        <f>SUM($I$2:I553)</f>
+        <v>36461.916666666672</v>
       </c>
     </row>
     <row r="554" spans="1:10" ht="12.75">
@@ -21710,8 +21710,8 @@
         <v>122.08333333333334</v>
       </c>
       <c r="J554" s="11">
-        <f>SUM($I$5:I554)</f>
-        <v>36498.125000000015</v>
+        <f>SUM($I$2:I554)</f>
+        <v>36584.000000000007</v>
       </c>
     </row>
     <row r="555" spans="1:10" ht="12.75">
@@ -21748,8 +21748,8 @@
         <v>117.08333333333334</v>
       </c>
       <c r="J555" s="11">
-        <f>SUM($I$5:I555)</f>
-        <v>36615.20833333335</v>
+        <f>SUM($I$2:I555)</f>
+        <v>36701.083333333343</v>
       </c>
     </row>
     <row r="556" spans="1:10" ht="12.75">
@@ -21786,8 +21786,8 @@
         <v>174.58333333333334</v>
       </c>
       <c r="J556" s="11">
-        <f>SUM($I$5:I556)</f>
-        <v>36789.791666666686</v>
+        <f>SUM($I$2:I556)</f>
+        <v>36875.666666666679</v>
       </c>
     </row>
     <row r="557" spans="1:10" ht="12.75">
@@ -21824,8 +21824,8 @@
         <v>87.083333333333357</v>
       </c>
       <c r="J557" s="11">
-        <f>SUM($I$5:I557)</f>
-        <v>36876.875000000022</v>
+        <f>SUM($I$2:I557)</f>
+        <v>36962.750000000015</v>
       </c>
     </row>
     <row r="558" spans="1:10" ht="12.75">
@@ -21862,8 +21862,8 @@
         <v>85</v>
       </c>
       <c r="J558" s="11">
-        <f>SUM($I$5:I558)</f>
-        <v>36961.875000000022</v>
+        <f>SUM($I$2:I558)</f>
+        <v>37047.750000000015</v>
       </c>
     </row>
     <row r="559" spans="1:10" ht="12.75">
@@ -21900,8 +21900,8 @@
         <v>30</v>
       </c>
       <c r="J559" s="11">
-        <f>SUM($I$5:I559)</f>
-        <v>36991.875000000022</v>
+        <f>SUM($I$2:I559)</f>
+        <v>37077.750000000015</v>
       </c>
     </row>
     <row r="560" spans="1:10" ht="12.75">
@@ -21938,8 +21938,8 @@
         <v>40.416666666666664</v>
       </c>
       <c r="J560" s="11">
-        <f>SUM($I$5:I560)</f>
-        <v>37032.291666666686</v>
+        <f>SUM($I$2:I560)</f>
+        <v>37118.166666666679</v>
       </c>
     </row>
     <row r="561" spans="1:10" ht="12.75">
@@ -21976,8 +21976,8 @@
         <v>92.5</v>
       </c>
       <c r="J561" s="11">
-        <f>SUM($I$5:I561)</f>
-        <v>37124.791666666686</v>
+        <f>SUM($I$2:I561)</f>
+        <v>37210.666666666679</v>
       </c>
     </row>
     <row r="562" spans="1:10" ht="12.75">
@@ -22014,8 +22014,8 @@
         <v>83.3333333333333</v>
       </c>
       <c r="J562" s="11">
-        <f>SUM($I$5:I562)</f>
-        <v>37208.125000000022</v>
+        <f>SUM($I$2:I562)</f>
+        <v>37294.000000000015</v>
       </c>
     </row>
     <row r="563" spans="1:10" ht="12.75">
@@ -22052,8 +22052,8 @@
         <v>252.08333333333334</v>
       </c>
       <c r="J563" s="11">
-        <f>SUM($I$5:I563)</f>
-        <v>37460.208333333358</v>
+        <f>SUM($I$2:I563)</f>
+        <v>37546.08333333335</v>
       </c>
     </row>
     <row r="564" spans="1:10" ht="12.75">
@@ -22090,8 +22090,8 @@
         <v>213.75000000000003</v>
       </c>
       <c r="J564" s="11">
-        <f>SUM($I$5:I564)</f>
-        <v>37673.958333333358</v>
+        <f>SUM($I$2:I564)</f>
+        <v>37759.83333333335</v>
       </c>
     </row>
     <row r="565" spans="1:10" ht="12.75">
@@ -22128,8 +22128,8 @@
         <v>52.5</v>
       </c>
       <c r="J565" s="11">
-        <f>SUM($I$5:I565)</f>
-        <v>37726.458333333358</v>
+        <f>SUM($I$2:I565)</f>
+        <v>37812.33333333335</v>
       </c>
     </row>
     <row r="566" spans="1:10" ht="12.75">
@@ -22166,8 +22166,8 @@
         <v>212.5</v>
       </c>
       <c r="J566" s="11">
-        <f>SUM($I$5:I566)</f>
-        <v>37938.958333333358</v>
+        <f>SUM($I$2:I566)</f>
+        <v>38024.83333333335</v>
       </c>
     </row>
     <row r="567" spans="1:10" ht="12.75">
@@ -22204,8 +22204,8 @@
         <v>27.916666666666668</v>
       </c>
       <c r="J567" s="11">
-        <f>SUM($I$5:I567)</f>
-        <v>37966.875000000022</v>
+        <f>SUM($I$2:I567)</f>
+        <v>38052.750000000015</v>
       </c>
     </row>
     <row r="568" spans="1:10" ht="12.75">
@@ -22242,8 +22242,8 @@
         <v>112.08333333333333</v>
       </c>
       <c r="J568" s="11">
-        <f>SUM($I$5:I568)</f>
-        <v>38078.958333333358</v>
+        <f>SUM($I$2:I568)</f>
+        <v>38164.83333333335</v>
       </c>
     </row>
     <row r="569" spans="1:10" ht="12.75">
@@ -22280,8 +22280,8 @@
         <v>81.666666666666643</v>
       </c>
       <c r="J569" s="11">
-        <f>SUM($I$5:I569)</f>
-        <v>38160.625000000022</v>
+        <f>SUM($I$2:I569)</f>
+        <v>38246.500000000015</v>
       </c>
     </row>
     <row r="570" spans="1:10" ht="12.75">
@@ -22318,8 +22318,8 @@
         <v>126.66666666666666</v>
       </c>
       <c r="J570" s="11">
-        <f>SUM($I$5:I570)</f>
-        <v>38287.291666666686</v>
+        <f>SUM($I$2:I570)</f>
+        <v>38373.166666666679</v>
       </c>
     </row>
     <row r="571" spans="1:10" ht="12.75">
@@ -22356,8 +22356,8 @@
         <v>119.16666666666667</v>
       </c>
       <c r="J571" s="11">
-        <f>SUM($I$5:I571)</f>
-        <v>38406.45833333335</v>
+        <f>SUM($I$2:I571)</f>
+        <v>38492.333333333343</v>
       </c>
     </row>
     <row r="572" spans="1:10" ht="12.75">
@@ -22394,8 +22394,8 @@
         <v>144.16666666666663</v>
       </c>
       <c r="J572" s="11">
-        <f>SUM($I$5:I572)</f>
-        <v>38550.625000000015</v>
+        <f>SUM($I$2:I572)</f>
+        <v>38636.500000000007</v>
       </c>
     </row>
     <row r="573" spans="1:10" ht="12.75">
@@ -22432,8 +22432,8 @@
         <v>103.75000000000001</v>
       </c>
       <c r="J573" s="11">
-        <f>SUM($I$5:I573)</f>
-        <v>38654.375000000015</v>
+        <f>SUM($I$2:I573)</f>
+        <v>38740.250000000007</v>
       </c>
     </row>
     <row r="574" spans="1:10" ht="12.75">
@@ -22470,8 +22470,8 @@
         <v>114.16666666666666</v>
       </c>
       <c r="J574" s="11">
-        <f>SUM($I$5:I574)</f>
-        <v>38768.541666666679</v>
+        <f>SUM($I$2:I574)</f>
+        <v>38854.416666666672</v>
       </c>
     </row>
     <row r="575" spans="1:10" ht="12.75">
@@ -22508,8 +22508,8 @@
         <v>131.25</v>
       </c>
       <c r="J575" s="11">
-        <f>SUM($I$5:I575)</f>
-        <v>38899.791666666679</v>
+        <f>SUM($I$2:I575)</f>
+        <v>38985.666666666672</v>
       </c>
     </row>
     <row r="576" spans="1:10" ht="12.75">
@@ -22546,8 +22546,8 @@
         <v>135.41666666666669</v>
       </c>
       <c r="J576" s="11">
-        <f>SUM($I$5:I576)</f>
-        <v>39035.208333333343</v>
+        <f>SUM($I$2:I576)</f>
+        <v>39121.083333333336</v>
       </c>
     </row>
     <row r="577" spans="1:10" ht="12.75">
@@ -22584,8 +22584,8 @@
         <v>161.66666666666666</v>
       </c>
       <c r="J577" s="11">
-        <f>SUM($I$5:I577)</f>
-        <v>39196.875000000007</v>
+        <f>SUM($I$2:I577)</f>
+        <v>39282.75</v>
       </c>
     </row>
     <row r="578" spans="1:10" ht="12.75">
@@ -22622,8 +22622,8 @@
         <v>118.33333333333336</v>
       </c>
       <c r="J578" s="11">
-        <f>SUM($I$5:I578)</f>
-        <v>39315.208333333343</v>
+        <f>SUM($I$2:I578)</f>
+        <v>39401.083333333336</v>
       </c>
     </row>
     <row r="579" spans="1:10" ht="12.75">
@@ -22660,8 +22660,8 @@
         <v>91.666666666666657</v>
       </c>
       <c r="J579" s="11">
-        <f>SUM($I$5:I579)</f>
-        <v>39406.875000000007</v>
+        <f>SUM($I$2:I579)</f>
+        <v>39492.75</v>
       </c>
     </row>
     <row r="580" spans="1:10" ht="12.75">
@@ -22698,8 +22698,8 @@
         <v>102.91666666666666</v>
       </c>
       <c r="J580" s="11">
-        <f>SUM($I$5:I580)</f>
-        <v>39509.791666666672</v>
+        <f>SUM($I$2:I580)</f>
+        <v>39595.666666666664</v>
       </c>
     </row>
     <row r="581" spans="1:10" ht="12.75">
@@ -22736,8 +22736,8 @@
         <v>32.083333333333336</v>
       </c>
       <c r="J581" s="11">
-        <f>SUM($I$5:I581)</f>
-        <v>39541.875000000007</v>
+        <f>SUM($I$2:I581)</f>
+        <v>39627.75</v>
       </c>
     </row>
     <row r="582" spans="1:10" ht="12.75">
@@ -22774,8 +22774,8 @@
         <v>114.99999999999999</v>
       </c>
       <c r="J582" s="11">
-        <f>SUM($I$5:I582)</f>
-        <v>39656.875000000007</v>
+        <f>SUM($I$2:I582)</f>
+        <v>39742.75</v>
       </c>
     </row>
     <row r="583" spans="1:10" ht="12.75">
@@ -22812,8 +22812,8 @@
         <v>63.333333333333329</v>
       </c>
       <c r="J583" s="11">
-        <f>SUM($I$5:I583)</f>
-        <v>39720.208333333343</v>
+        <f>SUM($I$2:I583)</f>
+        <v>39806.083333333336</v>
       </c>
     </row>
     <row r="584" spans="1:10" ht="12.75">
@@ -22850,8 +22850,8 @@
         <v>211.66666666666666</v>
       </c>
       <c r="J584" s="11">
-        <f>SUM($I$5:I584)</f>
-        <v>39931.875000000007</v>
+        <f>SUM($I$2:I584)</f>
+        <v>40017.75</v>
       </c>
     </row>
     <row r="585" spans="1:10" ht="12.75">
@@ -22888,8 +22888,8 @@
         <v>108.74999999999999</v>
       </c>
       <c r="J585" s="11">
-        <f>SUM($I$5:I585)</f>
-        <v>40040.625000000007</v>
+        <f>SUM($I$2:I585)</f>
+        <v>40126.5</v>
       </c>
     </row>
     <row r="586" spans="1:10" ht="12.75">
@@ -22926,8 +22926,8 @@
         <v>81.25</v>
       </c>
       <c r="J586" s="11">
-        <f>SUM($I$5:I586)</f>
-        <v>40121.875000000007</v>
+        <f>SUM($I$2:I586)</f>
+        <v>40207.75</v>
       </c>
     </row>
     <row r="587" spans="1:10" ht="12.75">
@@ -22964,8 +22964,8 @@
         <v>209.16666666666669</v>
       </c>
       <c r="J587" s="11">
-        <f>SUM($I$5:I587)</f>
-        <v>40331.041666666672</v>
+        <f>SUM($I$2:I587)</f>
+        <v>40416.916666666664</v>
       </c>
     </row>
     <row r="588" spans="1:10" ht="12.75">
@@ -23002,8 +23002,8 @@
         <v>165.83333333333331</v>
       </c>
       <c r="J588" s="11">
-        <f>SUM($I$5:I588)</f>
-        <v>40496.875000000007</v>
+        <f>SUM($I$2:I588)</f>
+        <v>40582.75</v>
       </c>
     </row>
     <row r="589" spans="1:10" ht="12.75">
@@ -23040,8 +23040,8 @@
         <v>197.91666666666669</v>
       </c>
       <c r="J589" s="11">
-        <f>SUM($I$5:I589)</f>
-        <v>40694.791666666672</v>
+        <f>SUM($I$2:I589)</f>
+        <v>40780.666666666664</v>
       </c>
     </row>
     <row r="590" spans="1:10" ht="12.75">
@@ -23078,8 +23078,8 @@
         <v>231.25</v>
       </c>
       <c r="J590" s="11">
-        <f>SUM($I$5:I590)</f>
-        <v>40926.041666666672</v>
+        <f>SUM($I$2:I590)</f>
+        <v>41011.916666666664</v>
       </c>
     </row>
     <row r="591" spans="1:10" ht="12.75">
@@ -23116,8 +23116,8 @@
         <v>62.5</v>
       </c>
       <c r="J591" s="11">
-        <f>SUM($I$5:I591)</f>
-        <v>40988.541666666672</v>
+        <f>SUM($I$2:I591)</f>
+        <v>41074.416666666664</v>
       </c>
     </row>
     <row r="592" spans="1:10" ht="12.75">
@@ -23154,8 +23154,8 @@
         <v>138.33333333333337</v>
       </c>
       <c r="J592" s="11">
-        <f>SUM($I$5:I592)</f>
-        <v>41126.875000000007</v>
+        <f>SUM($I$2:I592)</f>
+        <v>41212.75</v>
       </c>
     </row>
     <row r="593" spans="1:10" ht="12.75">
@@ -23192,8 +23192,8 @@
         <v>176.25000000000003</v>
       </c>
       <c r="J593" s="11">
-        <f>SUM($I$5:I593)</f>
-        <v>41303.125000000007</v>
+        <f>SUM($I$2:I593)</f>
+        <v>41389</v>
       </c>
     </row>
     <row r="594" spans="1:10" ht="12.75">
@@ -23230,8 +23230,8 @@
         <v>18.75</v>
       </c>
       <c r="J594" s="11">
-        <f>SUM($I$5:I594)</f>
-        <v>41321.875000000007</v>
+        <f>SUM($I$2:I594)</f>
+        <v>41407.75</v>
       </c>
     </row>
     <row r="595" spans="1:10" ht="12.75">
@@ -23268,8 +23268,8 @@
         <v>120</v>
       </c>
       <c r="J595" s="11">
-        <f>SUM($I$5:I595)</f>
-        <v>41441.875000000007</v>
+        <f>SUM($I$2:I595)</f>
+        <v>41527.75</v>
       </c>
     </row>
     <row r="596" spans="1:10" ht="12.75">
@@ -23306,8 +23306,8 @@
         <v>133.33333333333331</v>
       </c>
       <c r="J596" s="11">
-        <f>SUM($I$5:I596)</f>
-        <v>41575.208333333343</v>
+        <f>SUM($I$2:I596)</f>
+        <v>41661.083333333336</v>
       </c>
     </row>
     <row r="597" spans="1:10" ht="12.75">
@@ -23344,8 +23344,8 @@
         <v>136.25</v>
       </c>
       <c r="J597" s="11">
-        <f>SUM($I$5:I597)</f>
-        <v>41711.458333333343</v>
+        <f>SUM($I$2:I597)</f>
+        <v>41797.333333333336</v>
       </c>
     </row>
     <row r="598" spans="1:10" ht="12.75">
@@ -23382,8 +23382,8 @@
         <v>78.75</v>
       </c>
       <c r="J598" s="11">
-        <f>SUM($I$5:I598)</f>
-        <v>41790.208333333343</v>
+        <f>SUM($I$2:I598)</f>
+        <v>41876.083333333336</v>
       </c>
     </row>
     <row r="599" spans="1:10" ht="12.75">
@@ -23420,8 +23420,8 @@
         <v>107.5</v>
       </c>
       <c r="J599" s="11">
-        <f>SUM($I$5:I599)</f>
-        <v>41897.708333333343</v>
+        <f>SUM($I$2:I599)</f>
+        <v>41983.583333333336</v>
       </c>
     </row>
     <row r="600" spans="1:10" ht="12.75">
@@ -23458,8 +23458,8 @@
         <v>219.58333333333334</v>
       </c>
       <c r="J600" s="11">
-        <f>SUM($I$5:I600)</f>
-        <v>42117.291666666679</v>
+        <f>SUM($I$2:I600)</f>
+        <v>42203.166666666672</v>
       </c>
     </row>
     <row r="601" spans="1:10" ht="12.75">
@@ -23496,8 +23496,8 @@
         <v>157.08333333333334</v>
       </c>
       <c r="J601" s="11">
-        <f>SUM($I$5:I601)</f>
-        <v>42274.375000000015</v>
+        <f>SUM($I$2:I601)</f>
+        <v>42360.250000000007</v>
       </c>
     </row>
     <row r="602" spans="1:10" ht="12.75">
@@ -23534,8 +23534,8 @@
         <v>56.666666666666664</v>
       </c>
       <c r="J602" s="11">
-        <f>SUM($I$5:I602)</f>
-        <v>42331.041666666679</v>
+        <f>SUM($I$2:I602)</f>
+        <v>42416.916666666672</v>
       </c>
     </row>
     <row r="603" spans="1:10" ht="12.75">
@@ -23572,8 +23572,8 @@
         <v>43.75</v>
       </c>
       <c r="J603" s="11">
-        <f>SUM($I$5:I603)</f>
-        <v>42374.791666666679</v>
+        <f>SUM($I$2:I603)</f>
+        <v>42460.666666666672</v>
       </c>
     </row>
     <row r="604" spans="1:10" ht="12.75">
@@ -23610,8 +23610,8 @@
         <v>166.25</v>
       </c>
       <c r="J604" s="11">
-        <f>SUM($I$5:I604)</f>
-        <v>42541.041666666679</v>
+        <f>SUM($I$2:I604)</f>
+        <v>42626.916666666672</v>
       </c>
     </row>
     <row r="605" spans="1:10" ht="12.75">
@@ -23648,8 +23648,8 @@
         <v>193.75</v>
       </c>
       <c r="J605" s="11">
-        <f>SUM($I$5:I605)</f>
-        <v>42734.791666666679</v>
+        <f>SUM($I$2:I605)</f>
+        <v>42820.666666666672</v>
       </c>
     </row>
     <row r="606" spans="1:10" ht="12.75">
@@ -23686,8 +23686,8 @@
         <v>117.08333333333334</v>
       </c>
       <c r="J606" s="11">
-        <f>SUM($I$5:I606)</f>
-        <v>42851.875000000015</v>
+        <f>SUM($I$2:I606)</f>
+        <v>42937.750000000007</v>
       </c>
     </row>
     <row r="607" spans="1:10" ht="12.75">
@@ -23724,8 +23724,8 @@
         <v>43.333333333333336</v>
       </c>
       <c r="J607" s="11">
-        <f>SUM($I$5:I607)</f>
-        <v>42895.20833333335</v>
+        <f>SUM($I$2:I607)</f>
+        <v>42981.083333333343</v>
       </c>
     </row>
     <row r="608" spans="1:10" ht="12.75">
@@ -23762,8 +23762,8 @@
         <v>32.5</v>
       </c>
       <c r="J608" s="11">
-        <f>SUM($I$5:I608)</f>
-        <v>42927.70833333335</v>
+        <f>SUM($I$2:I608)</f>
+        <v>43013.583333333343</v>
       </c>
     </row>
     <row r="609" spans="1:10" ht="12.75">
@@ -23800,8 +23800,8 @@
         <v>118.33333333333333</v>
       </c>
       <c r="J609" s="11">
-        <f>SUM($I$5:I609)</f>
-        <v>43046.041666666686</v>
+        <f>SUM($I$2:I609)</f>
+        <v>43131.916666666679</v>
       </c>
     </row>
     <row r="610" spans="1:10" ht="12.75">
@@ -23838,8 +23838,8 @@
         <v>58.333333333333336</v>
       </c>
       <c r="J610" s="11">
-        <f>SUM($I$5:I610)</f>
-        <v>43104.375000000022</v>
+        <f>SUM($I$2:I610)</f>
+        <v>43190.250000000015</v>
       </c>
     </row>
     <row r="611" spans="1:10" ht="12.75">
@@ -23876,8 +23876,8 @@
         <v>77.916666666666671</v>
       </c>
       <c r="J611" s="11">
-        <f>SUM($I$5:I611)</f>
-        <v>43182.291666666686</v>
+        <f>SUM($I$2:I611)</f>
+        <v>43268.166666666679</v>
       </c>
     </row>
     <row r="612" spans="1:10" ht="12.75">
@@ -23914,8 +23914,8 @@
         <v>120</v>
       </c>
       <c r="J612" s="11">
-        <f>SUM($I$5:I612)</f>
-        <v>43302.291666666686</v>
+        <f>SUM($I$2:I612)</f>
+        <v>43388.166666666679</v>
       </c>
     </row>
     <row r="613" spans="1:10" ht="12.75">
@@ -23952,8 +23952,8 @@
         <v>82.916666666666671</v>
       </c>
       <c r="J613" s="11">
-        <f>SUM($I$5:I613)</f>
-        <v>43385.20833333335</v>
+        <f>SUM($I$2:I613)</f>
+        <v>43471.083333333343</v>
       </c>
     </row>
     <row r="614" spans="1:10" ht="12.75">
@@ -23990,8 +23990,8 @@
         <v>73.333333333333329</v>
       </c>
       <c r="J614" s="11">
-        <f>SUM($I$5:I614)</f>
-        <v>43458.541666666686</v>
+        <f>SUM($I$2:I614)</f>
+        <v>43544.416666666679</v>
       </c>
     </row>
     <row r="615" spans="1:10" ht="12.75">
@@ -24028,8 +24028,8 @@
         <v>137.5</v>
       </c>
       <c r="J615" s="11">
-        <f>SUM($I$5:I615)</f>
-        <v>43596.041666666686</v>
+        <f>SUM($I$2:I615)</f>
+        <v>43681.916666666679</v>
       </c>
     </row>
     <row r="616" spans="1:10" ht="12.75">
@@ -24066,8 +24066,8 @@
         <v>125.41666666666667</v>
       </c>
       <c r="J616" s="11">
-        <f>SUM($I$5:I616)</f>
-        <v>43721.45833333335</v>
+        <f>SUM($I$2:I616)</f>
+        <v>43807.333333333343</v>
       </c>
     </row>
     <row r="617" spans="1:10" ht="12.75">
@@ -24104,8 +24104,8 @@
         <v>113.75</v>
       </c>
       <c r="J617" s="11">
-        <f>SUM($I$5:I617)</f>
-        <v>43835.20833333335</v>
+        <f>SUM($I$2:I617)</f>
+        <v>43921.083333333343</v>
       </c>
     </row>
     <row r="618" spans="1:10" ht="12.75">
@@ -24142,8 +24142,8 @@
         <v>91.666666666666657</v>
       </c>
       <c r="J618" s="11">
-        <f>SUM($I$5:I618)</f>
-        <v>43926.875000000015</v>
+        <f>SUM($I$2:I618)</f>
+        <v>44012.750000000007</v>
       </c>
     </row>
     <row r="619" spans="1:10" ht="12.75">
@@ -24180,8 +24180,8 @@
         <v>98.75</v>
       </c>
       <c r="J619" s="11">
-        <f>SUM($I$5:I619)</f>
-        <v>44025.625000000015</v>
+        <f>SUM($I$2:I619)</f>
+        <v>44111.500000000007</v>
       </c>
     </row>
     <row r="620" spans="1:10" ht="12.75">
@@ -24218,8 +24218,8 @@
         <v>128.33333333333334</v>
       </c>
       <c r="J620" s="11">
-        <f>SUM($I$5:I620)</f>
-        <v>44153.95833333335</v>
+        <f>SUM($I$2:I620)</f>
+        <v>44239.833333333343</v>
       </c>
     </row>
     <row r="621" spans="1:10" ht="12.75">
@@ -24256,8 +24256,8 @@
         <v>103.33333333333334</v>
       </c>
       <c r="J621" s="11">
-        <f>SUM($I$5:I621)</f>
-        <v>44257.291666666686</v>
+        <f>SUM($I$2:I621)</f>
+        <v>44343.166666666679</v>
       </c>
     </row>
     <row r="622" spans="1:10" ht="12.75">
@@ -24294,8 +24294,8 @@
         <v>110.41666666666667</v>
       </c>
       <c r="J622" s="11">
-        <f>SUM($I$5:I622)</f>
-        <v>44367.70833333335</v>
+        <f>SUM($I$2:I622)</f>
+        <v>44453.583333333343</v>
       </c>
     </row>
     <row r="623" spans="1:10" ht="12.75">
@@ -24332,8 +24332,8 @@
         <v>63.333333333333329</v>
       </c>
       <c r="J623" s="11">
-        <f>SUM($I$5:I623)</f>
-        <v>44431.041666666686</v>
+        <f>SUM($I$2:I623)</f>
+        <v>44516.916666666679</v>
       </c>
     </row>
     <row r="624" spans="1:10" ht="12.75">
@@ -24370,8 +24370,8 @@
         <v>113.75</v>
       </c>
       <c r="J624" s="11">
-        <f>SUM($I$5:I624)</f>
-        <v>44544.791666666686</v>
+        <f>SUM($I$2:I624)</f>
+        <v>44630.666666666679</v>
       </c>
     </row>
     <row r="625" spans="1:10" ht="12.75">
@@ -24408,8 +24408,8 @@
         <v>118.33333333333333</v>
       </c>
       <c r="J625" s="11">
-        <f>SUM($I$5:I625)</f>
-        <v>44663.125000000022</v>
+        <f>SUM($I$2:I625)</f>
+        <v>44749.000000000015</v>
       </c>
     </row>
     <row r="626" spans="1:10" ht="12.75">
@@ -24446,8 +24446,8 @@
         <v>107.91666666666666</v>
       </c>
       <c r="J626" s="11">
-        <f>SUM($I$5:I626)</f>
-        <v>44771.041666666686</v>
+        <f>SUM($I$2:I626)</f>
+        <v>44856.916666666679</v>
       </c>
     </row>
     <row r="627" spans="1:10" ht="12.75">
@@ -25449,7 +25449,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B2" sqref="B2:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -25730,8 +25730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511715C2-8710-42EA-A7FE-B08466653F7D}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>